<commit_message>
data formatting and cleaning update
</commit_message>
<xml_diff>
--- a/code/output/data_price.xlsx
+++ b/code/output/data_price.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>name_prep_eng</t>
   </si>
@@ -22,9 +22,6 @@
     <t>price_kg_uah</t>
   </si>
   <si>
-    <t>Rice (raw)</t>
-  </si>
-  <si>
     <t>Rice (boiled)</t>
   </si>
   <si>
@@ -34,27 +31,18 @@
     <t>Rye bread (raw)</t>
   </si>
   <si>
-    <t>Beef (raw)</t>
-  </si>
-  <si>
     <t>Beef (boiled)</t>
   </si>
   <si>
     <t>Beef (roasted)</t>
   </si>
   <si>
-    <t>Pork (raw)</t>
-  </si>
-  <si>
     <t>Pork (boiled)</t>
   </si>
   <si>
     <t>Pork (roasted)</t>
   </si>
   <si>
-    <t>Chicken (raw)</t>
-  </si>
-  <si>
     <t>Chicken (boiled)</t>
   </si>
   <si>
@@ -67,18 +55,9 @@
     <t>Salo (roasted)</t>
   </si>
   <si>
-    <t>Wheat flour (raw)</t>
-  </si>
-  <si>
-    <t>Pasta (raw)</t>
-  </si>
-  <si>
     <t>Pasta (boiled)</t>
   </si>
   <si>
-    <t>Buckwheat (raw)</t>
-  </si>
-  <si>
     <t>Buckwheat (boiled)</t>
   </si>
   <si>
@@ -103,18 +82,12 @@
     <t>Sunflower oil (raw)</t>
   </si>
   <si>
-    <t>Eggs (raw)</t>
-  </si>
-  <si>
     <t>Eggs (boiled)</t>
   </si>
   <si>
     <t>Eggs (roasted)</t>
   </si>
   <si>
-    <t>Potatoes (raw)</t>
-  </si>
-  <si>
     <t>Potatoes (boiled)</t>
   </si>
   <si>
@@ -161,15 +134,6 @@
   </si>
   <si>
     <t>Walnuts (raw)</t>
-  </si>
-  <si>
-    <t>Oatmeal (raw)</t>
-  </si>
-  <si>
-    <t>Common mushrooms (raw)</t>
-  </si>
-  <si>
-    <t>Portabella mushrooms (raw)</t>
   </si>
   <si>
     <t>Figs (raw)</t>
@@ -560,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -579,7 +543,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>19.5</v>
+        <v>7.04</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -587,7 +551,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>7.04</v>
+        <v>12.37</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -595,7 +559,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>12.37</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -603,7 +567,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>12.25</v>
+        <v>179.41</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -611,7 +575,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>111.23</v>
+        <v>173.85</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -619,7 +583,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>179.41</v>
+        <v>171.47</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -627,7 +591,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>173.85</v>
+        <v>151.31</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -635,7 +599,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>102.86</v>
+        <v>73.81999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -643,7 +607,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>171.47</v>
+        <v>85.17</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -651,7 +615,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>151.31</v>
+        <v>60.06</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -659,7 +623,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>55.38</v>
+        <v>100.12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -667,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>73.81999999999999</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -675,7 +639,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>85.17</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -683,7 +647,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>60.06</v>
+        <v>72.68000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -691,7 +655,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>100.12</v>
+        <v>17.46</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -699,7 +663,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>9.68</v>
+        <v>45.73</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -707,7 +671,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>9.9</v>
+        <v>149.2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -715,7 +679,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>4.22</v>
+        <v>96.12</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -723,7 +687,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>22.8</v>
+        <v>15.58</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -731,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>6.11</v>
+        <v>32.76</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -739,7 +703,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>72.68000000000001</v>
+        <v>19.38</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -747,7 +711,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>17.46</v>
+        <v>25.83</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -755,7 +719,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>45.73</v>
+        <v>7.59</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -763,7 +727,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>149.2</v>
+        <v>9.130000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -771,7 +735,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>96.12</v>
+        <v>5.41</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -779,7 +743,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>15.58</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -787,7 +751,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>32.76</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -795,7 +759,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>19.38</v>
+        <v>7.74</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -803,7 +767,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>19.38</v>
+        <v>5.41</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -811,7 +775,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>25.83</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -819,7 +783,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>6.3</v>
+        <v>5.94</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -827,7 +791,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>7.59</v>
+        <v>8.02</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -835,7 +799,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>9.130000000000001</v>
+        <v>4.35</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -843,7 +807,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>5.41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -851,7 +815,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>5.88</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -859,7 +823,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>7.7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -867,7 +831,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>7.74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -875,7 +839,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>5.41</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -883,7 +847,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>5.7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -891,7 +855,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>5.94</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -899,7 +863,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>8.02</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -907,7 +871,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>4.35</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -915,7 +879,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -923,7 +887,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -939,7 +903,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>90</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -947,7 +911,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>220</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -955,7 +919,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>12.12</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -963,102 +927,6 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55">
-        <v>47.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62">
         <v>88</v>
       </c>
     </row>

</xml_diff>